<commit_message>
Added Lineage key to bank branches
</commit_message>
<xml_diff>
--- a/Dummy Data/Dim_Branch.xlsx
+++ b/Dummy Data/Dim_Branch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem2\Data Warehousing\assigment\Loan-Data-Warehouse\Dummy Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC41D6F-4B4D-4F5C-89D1-0BEB093B9EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22804BF-1665-4FEC-A825-157C4B16B1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
   <si>
     <t>Branch Name</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>_Source Key</t>
+  </si>
+  <si>
+    <t>Lineage Key</t>
   </si>
 </sst>
 </file>
@@ -571,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:L168"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +590,8 @@
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -620,6 +625,9 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -652,9 +660,12 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
       <c r="L2" t="str">
-        <f t="shared" ref="L2:L33" si="0">"INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;",'"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"');"</f>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303010,'ASIFABAD','564567',51,'501-10,000','Rural','Jowai','Meghalaya','India');</v>
+        <f>"INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES ("&amp;B2&amp;",'"&amp;C2&amp;"','"&amp;D2&amp;"',"&amp;E2&amp;",'"&amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"',"&amp;K2&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303010,'ASIFABAD','564567',51,'501-10,000','Rural','Jowai','Meghalaya','India',2);</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -688,9 +699,12 @@
       <c r="J3" t="s">
         <v>12</v>
       </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
       <c r="L3" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303026,'BOATH','675675',38,'501-10,000','Rural','Arvi','Maharashtra','India');</v>
+        <f t="shared" ref="L3:L21" si="0">"INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES ("&amp;B3&amp;",'"&amp;C3&amp;"','"&amp;D3&amp;"',"&amp;E3&amp;",'"&amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"',"&amp;K3&amp;");"</f>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303026,'BOATH','675675',38,'501-10,000','Rural','Arvi','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -724,9 +738,12 @@
       <c r="J4" t="s">
         <v>12</v>
       </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303183,'CHINNOR','400016',97,'501-10,000','Rural','Mumbai','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303183,'CHINNOR','400016',97,'501-10,000','Rural','Mumbai','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -760,9 +777,12 @@
       <c r="J5" t="s">
         <v>12</v>
       </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303190,'KHANAPUR','673639',45,'501-10,000','Corporate','Kozhikode','Kerala','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303190,'KHANAPUR','673639',45,'501-10,000','Corporate','Kozhikode','Kerala','India',2);</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -796,9 +816,12 @@
       <c r="J6" t="s">
         <v>12</v>
       </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303215,'LUXETTIPET','411006',66,'501-10,000','Personal','Pune','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303215,'LUXETTIPET','411006',66,'501-10,000','Personal','Pune','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -832,9 +855,12 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303597,'MUDHOL AP','679103',43,'501-10,000','Corporate','Ottappalam','Kerala','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303597,'MUDHOL AP','679103',43,'501-10,000','Corporate','Ottappalam','Kerala','India',2);</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -868,9 +894,12 @@
       <c r="J8" t="s">
         <v>12</v>
       </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303027,'SIRPUR TOWN','765756',93,'501-10,000','Rural','Kakching','Manipur','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303027,'SIRPUR TOWN','765756',93,'501-10,000','Rural','Kakching','Manipur','India',2);</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -904,9 +933,12 @@
       <c r="J9" t="s">
         <v>12</v>
       </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303037,'UTNOOR','400093',64,'501-10,000','Personal','Mumbai','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303037,'UTNOOR','400093',64,'501-10,000','Personal','Mumbai','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -940,9 +972,12 @@
       <c r="J10" t="s">
         <v>12</v>
       </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303096,'MAIN BR','400093',42,'501-10,000','Corporate','Mumbai','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303096,'MAIN BR','400093',42,'501-10,000','Corporate','Mumbai','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -976,9 +1011,12 @@
       <c r="J11" t="s">
         <v>12</v>
       </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303105,'JAGTIAL','646467',52,'501-10,000','Personal','Deoghar','Jharkhand','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303105,'JAGTIAL','646467',52,'501-10,000','Personal','Deoghar','Jharkhand','India',2);</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1012,9 +1050,12 @@
       <c r="J12" t="s">
         <v>12</v>
       </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303112,'JAMMIKUNTA','400088',73,'501-10,000','Personal','Adoni','Andhra Pradesh','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303112,'JAMMIKUNTA','400088',73,'501-10,000','Personal','Adoni','Andhra Pradesh','India',2);</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1048,9 +1089,12 @@
       <c r="J13" t="s">
         <v>12</v>
       </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303015,'KORATLA','503217',44,'501-10,000','Rural','Abhayapuri','Telangana','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303015,'KORATLA','503217',44,'501-10,000','Rural','Abhayapuri','Telangana','India',2);</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1084,9 +1128,12 @@
       <c r="J14" t="s">
         <v>12</v>
       </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303031,'PEDDAPALLI','441904',37,'501-10,000','Personal','Bhandara','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303031,'PEDDAPALLI','441904',37,'501-10,000','Personal','Bhandara','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1120,9 +1167,12 @@
       <c r="J15" t="s">
         <v>12</v>
       </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303231,'RAMAGUNDEM','121002',42,'501-10,000','Rural','Faridabad','Haryana','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303231,'RAMAGUNDEM','121002',42,'501-10,000','Rural','Faridabad','Haryana','India',2);</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -1156,9 +1206,12 @@
       <c r="J16" t="s">
         <v>12</v>
       </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303237,'SIRCILLA','272155',70,'501-10,000','Personal','Gorakhpur','Uttar Pradesh','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303237,'SIRCILLA','272155',70,'501-10,000','Personal','Gorakhpur','Uttar Pradesh','India',2);</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -1192,9 +1245,12 @@
       <c r="J17" t="s">
         <v>12</v>
       </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303244,'DHARMAPURI','844102',39,'501-10,000','Personal','Hajipur','Bihar','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303244,'DHARMAPURI','844102',39,'501-10,000','Personal','Hajipur','Bihar','India',2);</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -1228,9 +1284,12 @@
       <c r="J18" t="s">
         <v>12</v>
       </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303020,'GANGADHARA','272301',40,'0-500','Personal','Gorakhpur','Uttar Pradesh','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303020,'GANGADHARA','272301',40,'0-500','Personal','Gorakhpur','Uttar Pradesh','India',2);</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1264,9 +1323,12 @@
       <c r="J19" t="s">
         <v>12</v>
       </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303129,'HUZURABAD','263139',37,'501-10,000','Personal','Haldwani','Uttarakhand','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303129,'HUZURABAD','263139',37,'501-10,000','Personal','Haldwani','Uttarakhand','India',2);</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -1300,9 +1362,12 @@
       <c r="J20" t="s">
         <v>12</v>
       </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
       <c r="L20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303155,'MANTHANI','332701',91,'501-10,000','Rural','Sikar','Rajasthan','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303155,'MANTHANI','332701',91,'501-10,000','Rural','Sikar','Rajasthan','India',2);</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -1336,9 +1401,12 @@
       <c r="J21" t="s">
         <v>12</v>
       </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
       <c r="L21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country]) VALUES (303184,'METPALLY','414603',100,'501-10,000','Rural','Ahmednagar','Maharashtra','India');</v>
+        <v>INSERT into [dbo].[Dim_Branch] ([_Source Key], [Branch Name], [Branch PINCODE], [Number of Employees], [Number of Customers], [Branch Type], [City], [State], [Country], [Lineage Key]) VALUES (303184,'METPALLY','414603',100,'501-10,000','Rural','Ahmednagar','Maharashtra','India',2);</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>